<commit_message>
falta unir el archivo excel del final con los docs
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="8_{CC3E9899-0839-4122-9C1F-71EEB74DA066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CAD7218-622F-4954-9961-BBF076759D60}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{CC3E9899-0839-4122-9C1F-71EEB74DA066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FC53538-F9F2-4246-9F1E-EBC1CE234E90}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="570" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{91CFA281-0435-4FD3-9986-03D61E002608}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{91CFA281-0435-4FD3-9986-03D61E002608}"/>
   </bookViews>
   <sheets>
     <sheet name="Rutas" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>/PDDPROD</t>
   </si>
   <si>
-    <t>D:\Program Files (x86)\ERPSAP\SAPgui\saplogon.exe</t>
-  </si>
-  <si>
     <t>Usuario</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>MIGRACIONES SGV DICIEMBRE 2022 28.12.2022</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)\SAP\FrontEnd\SAPgui\saplogon.exe</t>
   </si>
 </sst>
 </file>
@@ -302,10 +302,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -607,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288CF779-B90E-47AA-B022-B9419930CC24}">
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -635,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D572AF7-C0B1-48C5-8294-DB042ACF598C}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -647,7 +643,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -655,7 +651,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -663,7 +659,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
@@ -694,10 +690,10 @@
     <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bot5 GUI terminando el bot
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/Bot5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="8_{CC3E9899-0839-4122-9C1F-71EEB74DA066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06370C05-C167-465E-9F69-017CEE749B83}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="8_{CC3E9899-0839-4122-9C1F-71EEB74DA066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29B8438D-7288-4E9B-B969-DF637EEF23CE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{91CFA281-0435-4FD3-9986-03D61E002608}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Path SAP logon</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Cntdad feriados</t>
+  </si>
+  <si>
+    <t>31.01.2023</t>
   </si>
 </sst>
 </file>
@@ -322,6 +325,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -613,7 +620,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -652,7 +659,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,13 +697,17 @@
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Bot5 GUI beta terminada
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="8_{CC3E9899-0839-4122-9C1F-71EEB74DA066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29B8438D-7288-4E9B-B969-DF637EEF23CE}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="8_{CC3E9899-0839-4122-9C1F-71EEB74DA066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4FDE1BC-0F96-4177-8A45-C7B82A3A8564}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{91CFA281-0435-4FD3-9986-03D61E002608}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Path SAP logon</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Cntdad feriados</t>
-  </si>
-  <si>
-    <t>31.01.2023</t>
   </si>
 </sst>
 </file>
@@ -325,10 +322,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -620,7 +613,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -659,7 +652,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,17 +690,13 @@
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4">
-        <v>10</v>
-      </c>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Bot5 GUI no había error del bot
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/Bot5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="167" documentId="8_{CC3E9899-0839-4122-9C1F-71EEB74DA066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4FDE1BC-0F96-4177-8A45-C7B82A3A8564}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="8_{CC3E9899-0839-4122-9C1F-71EEB74DA066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59446D07-D0EC-4103-9099-B6667A9F3F2F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{91CFA281-0435-4FD3-9986-03D61E002608}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{91CFA281-0435-4FD3-9986-03D61E002608}"/>
   </bookViews>
   <sheets>
     <sheet name="Rutas" sheetId="1" r:id="rId1"/>
@@ -652,7 +652,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +721,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bot5 GUI migraciones con nuevo formato implementado
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/Bot5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="8_{CC3E9899-0839-4122-9C1F-71EEB74DA066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1064A86C-9A86-4912-94D5-2C9702F518B0}"/>
+  <xr:revisionPtr revIDLastSave="188" documentId="8_{CC3E9899-0839-4122-9C1F-71EEB74DA066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86012845-40E5-4F83-BA4B-35EE828FB78A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{91CFA281-0435-4FD3-9986-03D61E002608}"/>
   </bookViews>
@@ -81,7 +81,7 @@
     <t>Cntdad feriados</t>
   </si>
   <si>
-    <t>MIGRACIONES SGV FEBRERO 2023 28.02.2023</t>
+    <t>MIGRACIONES SGV MARZO 2023 15.03.2023 BOOT 5</t>
   </si>
 </sst>
 </file>
@@ -653,13 +653,13 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>